<commit_message>
Update tournament analysis file
</commit_message>
<xml_diff>
--- a/data/Rivals1TournamentsAnalysis.xlsx
+++ b/data/Rivals1TournamentsAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlmon\Documents\GitHub\rivals-blog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA155DC-A82E-4873-99E5-8D9290E560F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A8F47D-C1F1-43CF-A49D-3FD80A04768F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{40EF91EA-8845-4BB8-88F3-89A70BCD1D65}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1368,14 +1368,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4047,21 +4046,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{ACAD4DCB-C46A-43E3-A436-186B1BC8423B}" name="Season_1" displayName="Season_1" ref="A1:P128" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:P128" xr:uid="{ACAD4DCB-C46A-43E3-A436-186B1BC8423B}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="6">
       <filters>
-        <filter val="CakeAssault"/>
-        <filter val="Dank Fornasty"/>
-        <filter val="Sam"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="15">
-      <filters>
-        <filter val="Show"/>
+        <filter val="Blue"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4085,7 +4072,7 @@
     <tableColumn id="14" xr3:uid="{66A1F28D-34AC-483E-87F0-507ACF3DD516}" uniqueName="14" name="Eighth" queryTableFieldId="14" dataDxfId="1"/>
     <tableColumn id="15" xr3:uid="{8D5CCE6F-A8B0-4071-847F-4C1CE40F277E}" uniqueName="15" name="Season" queryTableFieldId="15"/>
     <tableColumn id="16" xr3:uid="{7EA349DA-14D0-4B94-AB63-C43195C2B92F}" uniqueName="16" name="Player Filter" queryTableFieldId="16" dataDxfId="0">
-      <calculatedColumnFormula array="1">IF(SUM(COUNTIF(G2:N2, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</calculatedColumnFormula>
+      <calculatedColumnFormula array="1">IF(SUM(COUNTIF(G2:N2, {""}))&gt;0, "Show", "Hide")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4411,8 +4398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F684C4A-424F-47AF-A0CE-EEA276FC90B2}">
   <dimension ref="A1:R128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4489,7 +4476,7 @@
       </c>
       <c r="R1">
         <f>SUBTOTAL(3, A2:A200)</f>
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4538,8 +4525,8 @@
       <c r="O2" t="s">
         <v>395</v>
       </c>
-      <c r="P2" s="4" t="str" cm="1">
-        <f t="array" ref="P2">IF(SUM(COUNTIF(G2:N2, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P2" t="str" cm="1">
+        <f t="array" ref="P2">IF(SUM(COUNTIF(G2:N2, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -4589,8 +4576,8 @@
       <c r="O3" t="s">
         <v>397</v>
       </c>
-      <c r="P3" s="4" t="str" cm="1">
-        <f t="array" ref="P3">IF(SUM(COUNTIF(G3:N3, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P3" t="str" cm="1">
+        <f t="array" ref="P3">IF(SUM(COUNTIF(G3:N3, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -4640,9 +4627,9 @@
       <c r="O4" t="s">
         <v>400</v>
       </c>
-      <c r="P4" s="4" t="str" cm="1">
-        <f t="array" ref="P4">IF(SUM(COUNTIF(G4:N4, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P4" t="str" cm="1">
+        <f t="array" ref="P4">IF(SUM(COUNTIF(G4:N4, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4691,9 +4678,9 @@
       <c r="O5" t="s">
         <v>400</v>
       </c>
-      <c r="P5" s="4" t="str" cm="1">
-        <f t="array" ref="P5">IF(SUM(COUNTIF(G5:N5, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P5" t="str" cm="1">
+        <f t="array" ref="P5">IF(SUM(COUNTIF(G5:N5, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4742,9 +4729,9 @@
       <c r="O6" t="s">
         <v>401</v>
       </c>
-      <c r="P6" s="4" t="str" cm="1">
-        <f t="array" ref="P6">IF(SUM(COUNTIF(G6:N6, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P6" t="str" cm="1">
+        <f t="array" ref="P6">IF(SUM(COUNTIF(G6:N6, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4793,8 +4780,8 @@
       <c r="O7" t="s">
         <v>399</v>
       </c>
-      <c r="P7" s="4" t="str" cm="1">
-        <f t="array" ref="P7">IF(SUM(COUNTIF(G7:N7, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P7" t="str" cm="1">
+        <f t="array" ref="P7">IF(SUM(COUNTIF(G7:N7, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -4844,8 +4831,8 @@
       <c r="O8" t="s">
         <v>400</v>
       </c>
-      <c r="P8" s="4" t="str" cm="1">
-        <f t="array" ref="P8">IF(SUM(COUNTIF(G8:N8, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P8" t="str" cm="1">
+        <f t="array" ref="P8">IF(SUM(COUNTIF(G8:N8, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -4895,9 +4882,9 @@
       <c r="O9" t="s">
         <v>396</v>
       </c>
-      <c r="P9" s="4" t="str" cm="1">
-        <f t="array" ref="P9">IF(SUM(COUNTIF(G9:N9, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P9" t="str" cm="1">
+        <f t="array" ref="P9">IF(SUM(COUNTIF(G9:N9, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4946,9 +4933,9 @@
       <c r="O10" t="s">
         <v>400</v>
       </c>
-      <c r="P10" s="4" t="str" cm="1">
-        <f t="array" ref="P10">IF(SUM(COUNTIF(G10:N10, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P10" t="str" cm="1">
+        <f t="array" ref="P10">IF(SUM(COUNTIF(G10:N10, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4997,8 +4984,8 @@
       <c r="O11" t="s">
         <v>396</v>
       </c>
-      <c r="P11" s="4" t="str" cm="1">
-        <f t="array" ref="P11">IF(SUM(COUNTIF(G11:N11, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P11" t="str" cm="1">
+        <f t="array" ref="P11">IF(SUM(COUNTIF(G11:N11, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -5048,12 +5035,12 @@
       <c r="O12" t="s">
         <v>399</v>
       </c>
-      <c r="P12" s="4" t="str" cm="1">
-        <f t="array" ref="P12">IF(SUM(COUNTIF(G12:N12, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P12" t="str" cm="1">
+        <f t="array" ref="P12">IF(SUM(COUNTIF(G12:N12, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>388</v>
       </c>
@@ -5099,9 +5086,9 @@
       <c r="O13" t="s">
         <v>400</v>
       </c>
-      <c r="P13" s="4" t="str" cm="1">
-        <f t="array" ref="P13">IF(SUM(COUNTIF(G13:N13, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P13" t="str" cm="1">
+        <f t="array" ref="P13">IF(SUM(COUNTIF(G13:N13, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -5150,9 +5137,9 @@
       <c r="O14" t="s">
         <v>401</v>
       </c>
-      <c r="P14" s="4" t="str" cm="1">
-        <f t="array" ref="P14">IF(SUM(COUNTIF(G14:N14, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P14" t="str" cm="1">
+        <f t="array" ref="P14">IF(SUM(COUNTIF(G14:N14, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -5201,12 +5188,12 @@
       <c r="O15" t="s">
         <v>396</v>
       </c>
-      <c r="P15" s="4" t="str" cm="1">
-        <f t="array" ref="P15">IF(SUM(COUNTIF(G15:N15, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P15" t="str" cm="1">
+        <f t="array" ref="P15">IF(SUM(COUNTIF(G15:N15, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -5252,9 +5239,9 @@
       <c r="O16" t="s">
         <v>402</v>
       </c>
-      <c r="P16" s="4" t="str" cm="1">
-        <f t="array" ref="P16">IF(SUM(COUNTIF(G16:N16, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P16" t="str" cm="1">
+        <f t="array" ref="P16">IF(SUM(COUNTIF(G16:N16, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5303,9 +5290,9 @@
       <c r="O17" t="s">
         <v>400</v>
       </c>
-      <c r="P17" s="4" t="str" cm="1">
-        <f t="array" ref="P17">IF(SUM(COUNTIF(G17:N17, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P17" t="str" cm="1">
+        <f t="array" ref="P17">IF(SUM(COUNTIF(G17:N17, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5354,8 +5341,8 @@
       <c r="O18" t="s">
         <v>396</v>
       </c>
-      <c r="P18" s="4" t="str" cm="1">
-        <f t="array" ref="P18">IF(SUM(COUNTIF(G18:N18, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P18" t="str" cm="1">
+        <f t="array" ref="P18">IF(SUM(COUNTIF(G18:N18, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -5405,9 +5392,9 @@
       <c r="O19" t="s">
         <v>398</v>
       </c>
-      <c r="P19" s="4" t="str" cm="1">
-        <f t="array" ref="P19">IF(SUM(COUNTIF(G19:N19, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P19" t="str" cm="1">
+        <f t="array" ref="P19">IF(SUM(COUNTIF(G19:N19, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5456,8 +5443,8 @@
       <c r="O20" t="s">
         <v>401</v>
       </c>
-      <c r="P20" s="4" t="str" cm="1">
-        <f t="array" ref="P20">IF(SUM(COUNTIF(G20:N20, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P20" t="str" cm="1">
+        <f t="array" ref="P20">IF(SUM(COUNTIF(G20:N20, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -5507,8 +5494,8 @@
       <c r="O21" t="s">
         <v>401</v>
       </c>
-      <c r="P21" s="4" t="str" cm="1">
-        <f t="array" ref="P21">IF(SUM(COUNTIF(G21:N21, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P21" t="str" cm="1">
+        <f t="array" ref="P21">IF(SUM(COUNTIF(G21:N21, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -5558,12 +5545,12 @@
       <c r="O22" t="s">
         <v>397</v>
       </c>
-      <c r="P22" s="4" t="str" cm="1">
-        <f t="array" ref="P22">IF(SUM(COUNTIF(G22:N22, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P22" t="str" cm="1">
+        <f t="array" ref="P22">IF(SUM(COUNTIF(G22:N22, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>320</v>
       </c>
@@ -5609,9 +5596,9 @@
       <c r="O23" t="s">
         <v>397</v>
       </c>
-      <c r="P23" s="4" t="str" cm="1">
-        <f t="array" ref="P23">IF(SUM(COUNTIF(G23:N23, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P23" t="str" cm="1">
+        <f t="array" ref="P23">IF(SUM(COUNTIF(G23:N23, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5660,9 +5647,9 @@
       <c r="O24" t="s">
         <v>399</v>
       </c>
-      <c r="P24" s="4" t="str" cm="1">
-        <f t="array" ref="P24">IF(SUM(COUNTIF(G24:N24, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P24" t="str" cm="1">
+        <f t="array" ref="P24">IF(SUM(COUNTIF(G24:N24, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5711,12 +5698,12 @@
       <c r="O25" t="s">
         <v>399</v>
       </c>
-      <c r="P25" s="4" t="str" cm="1">
-        <f t="array" ref="P25">IF(SUM(COUNTIF(G25:N25, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P25" t="str" cm="1">
+        <f t="array" ref="P25">IF(SUM(COUNTIF(G25:N25, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -5762,12 +5749,12 @@
       <c r="O26" t="s">
         <v>402</v>
       </c>
-      <c r="P26" s="4" t="str" cm="1">
-        <f t="array" ref="P26">IF(SUM(COUNTIF(G26:N26, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P26" t="str" cm="1">
+        <f t="array" ref="P26">IF(SUM(COUNTIF(G26:N26, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -5813,12 +5800,12 @@
       <c r="O27" t="s">
         <v>403</v>
       </c>
-      <c r="P27" s="4" t="str" cm="1">
-        <f t="array" ref="P27">IF(SUM(COUNTIF(G27:N27, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P27" t="str" cm="1">
+        <f t="array" ref="P27">IF(SUM(COUNTIF(G27:N27, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -5864,9 +5851,9 @@
       <c r="O28" t="s">
         <v>401</v>
       </c>
-      <c r="P28" s="4" t="str" cm="1">
-        <f t="array" ref="P28">IF(SUM(COUNTIF(G28:N28, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P28" t="str" cm="1">
+        <f t="array" ref="P28">IF(SUM(COUNTIF(G28:N28, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5915,9 +5902,9 @@
       <c r="O29" t="s">
         <v>399</v>
       </c>
-      <c r="P29" s="4" t="str" cm="1">
-        <f t="array" ref="P29">IF(SUM(COUNTIF(G29:N29, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P29" t="str" cm="1">
+        <f t="array" ref="P29">IF(SUM(COUNTIF(G29:N29, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -5966,9 +5953,9 @@
       <c r="O30" t="s">
         <v>403</v>
       </c>
-      <c r="P30" s="4" t="str" cm="1">
-        <f t="array" ref="P30">IF(SUM(COUNTIF(G30:N30, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P30" t="str" cm="1">
+        <f t="array" ref="P30">IF(SUM(COUNTIF(G30:N30, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6017,12 +6004,12 @@
       <c r="O31" t="s">
         <v>396</v>
       </c>
-      <c r="P31" s="4" t="str" cm="1">
-        <f t="array" ref="P31">IF(SUM(COUNTIF(G31:N31, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P31" t="str" cm="1">
+        <f t="array" ref="P31">IF(SUM(COUNTIF(G31:N31, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -6068,9 +6055,9 @@
       <c r="O32" t="s">
         <v>401</v>
       </c>
-      <c r="P32" s="4" t="str" cm="1">
-        <f t="array" ref="P32">IF(SUM(COUNTIF(G32:N32, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P32" t="str" cm="1">
+        <f t="array" ref="P32">IF(SUM(COUNTIF(G32:N32, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6119,8 +6106,8 @@
       <c r="O33" t="s">
         <v>398</v>
       </c>
-      <c r="P33" s="4" t="str" cm="1">
-        <f t="array" ref="P33">IF(SUM(COUNTIF(G33:N33, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P33" t="str" cm="1">
+        <f t="array" ref="P33">IF(SUM(COUNTIF(G33:N33, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -6170,8 +6157,8 @@
       <c r="O34" t="s">
         <v>399</v>
       </c>
-      <c r="P34" s="4" t="str" cm="1">
-        <f t="array" ref="P34">IF(SUM(COUNTIF(G34:N34, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P34" t="str" cm="1">
+        <f t="array" ref="P34">IF(SUM(COUNTIF(G34:N34, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -6221,8 +6208,8 @@
       <c r="O35" t="s">
         <v>396</v>
       </c>
-      <c r="P35" s="4" t="str" cm="1">
-        <f t="array" ref="P35">IF(SUM(COUNTIF(G35:N35, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P35" t="str" cm="1">
+        <f t="array" ref="P35">IF(SUM(COUNTIF(G35:N35, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -6272,9 +6259,9 @@
       <c r="O36" t="s">
         <v>403</v>
       </c>
-      <c r="P36" s="4" t="str" cm="1">
-        <f t="array" ref="P36">IF(SUM(COUNTIF(G36:N36, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P36" t="str" cm="1">
+        <f t="array" ref="P36">IF(SUM(COUNTIF(G36:N36, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6323,12 +6310,12 @@
       <c r="O37" t="s">
         <v>397</v>
       </c>
-      <c r="P37" s="4" t="str" cm="1">
-        <f t="array" ref="P37">IF(SUM(COUNTIF(G37:N37, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P37" t="str" cm="1">
+        <f t="array" ref="P37">IF(SUM(COUNTIF(G37:N37, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>351</v>
       </c>
@@ -6374,9 +6361,9 @@
       <c r="O38" t="s">
         <v>398</v>
       </c>
-      <c r="P38" s="4" t="str" cm="1">
-        <f t="array" ref="P38">IF(SUM(COUNTIF(G38:N38, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P38" t="str" cm="1">
+        <f t="array" ref="P38">IF(SUM(COUNTIF(G38:N38, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6425,9 +6412,9 @@
       <c r="O39" t="s">
         <v>397</v>
       </c>
-      <c r="P39" s="4" t="str" cm="1">
-        <f t="array" ref="P39">IF(SUM(COUNTIF(G39:N39, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P39" t="str" cm="1">
+        <f t="array" ref="P39">IF(SUM(COUNTIF(G39:N39, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6476,8 +6463,8 @@
       <c r="O40" t="s">
         <v>397</v>
       </c>
-      <c r="P40" s="4" t="str" cm="1">
-        <f t="array" ref="P40">IF(SUM(COUNTIF(G40:N40, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P40" t="str" cm="1">
+        <f t="array" ref="P40">IF(SUM(COUNTIF(G40:N40, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -6527,12 +6514,12 @@
       <c r="O41" t="s">
         <v>397</v>
       </c>
-      <c r="P41" s="4" t="str" cm="1">
-        <f t="array" ref="P41">IF(SUM(COUNTIF(G41:N41, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P41" t="str" cm="1">
+        <f t="array" ref="P41">IF(SUM(COUNTIF(G41:N41, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -6578,9 +6565,9 @@
       <c r="O42" t="s">
         <v>402</v>
       </c>
-      <c r="P42" s="4" t="str" cm="1">
-        <f t="array" ref="P42">IF(SUM(COUNTIF(G42:N42, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P42" t="str" cm="1">
+        <f t="array" ref="P42">IF(SUM(COUNTIF(G42:N42, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6629,12 +6616,12 @@
       <c r="O43" t="s">
         <v>399</v>
       </c>
-      <c r="P43" s="4" t="str" cm="1">
-        <f t="array" ref="P43">IF(SUM(COUNTIF(G43:N43, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P43" t="str" cm="1">
+        <f t="array" ref="P43">IF(SUM(COUNTIF(G43:N43, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -6680,12 +6667,12 @@
       <c r="O44" t="s">
         <v>402</v>
       </c>
-      <c r="P44" s="4" t="str" cm="1">
-        <f t="array" ref="P44">IF(SUM(COUNTIF(G44:N44, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P44" t="str" cm="1">
+        <f t="array" ref="P44">IF(SUM(COUNTIF(G44:N44, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>313</v>
       </c>
@@ -6731,12 +6718,12 @@
       <c r="O45" t="s">
         <v>397</v>
       </c>
-      <c r="P45" s="4" t="str" cm="1">
-        <f t="array" ref="P45">IF(SUM(COUNTIF(G45:N45, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P45" t="str" cm="1">
+        <f t="array" ref="P45">IF(SUM(COUNTIF(G45:N45, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>296</v>
       </c>
@@ -6782,12 +6769,12 @@
       <c r="O46" t="s">
         <v>396</v>
       </c>
-      <c r="P46" s="4" t="str" cm="1">
-        <f t="array" ref="P46">IF(SUM(COUNTIF(G46:N46, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P46" t="str" cm="1">
+        <f t="array" ref="P46">IF(SUM(COUNTIF(G46:N46, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>303</v>
       </c>
@@ -6833,9 +6820,9 @@
       <c r="O47" t="s">
         <v>397</v>
       </c>
-      <c r="P47" s="4" t="str" cm="1">
-        <f t="array" ref="P47">IF(SUM(COUNTIF(G47:N47, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P47" t="str" cm="1">
+        <f t="array" ref="P47">IF(SUM(COUNTIF(G47:N47, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6884,12 +6871,12 @@
       <c r="O48" t="s">
         <v>396</v>
       </c>
-      <c r="P48" s="4" t="str" cm="1">
-        <f t="array" ref="P48">IF(SUM(COUNTIF(G48:N48, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P48" t="str" cm="1">
+        <f t="array" ref="P48">IF(SUM(COUNTIF(G48:N48, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>279</v>
       </c>
@@ -6935,9 +6922,9 @@
       <c r="O49" t="s">
         <v>396</v>
       </c>
-      <c r="P49" s="4" t="str" cm="1">
-        <f t="array" ref="P49">IF(SUM(COUNTIF(G49:N49, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P49" t="str" cm="1">
+        <f t="array" ref="P49">IF(SUM(COUNTIF(G49:N49, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -6986,9 +6973,9 @@
       <c r="O50" t="s">
         <v>398</v>
       </c>
-      <c r="P50" s="4" t="str" cm="1">
-        <f t="array" ref="P50">IF(SUM(COUNTIF(G50:N50, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P50" t="str" cm="1">
+        <f t="array" ref="P50">IF(SUM(COUNTIF(G50:N50, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7037,12 +7024,12 @@
       <c r="O51" t="s">
         <v>397</v>
       </c>
-      <c r="P51" s="4" t="str" cm="1">
-        <f t="array" ref="P51">IF(SUM(COUNTIF(G51:N51, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P51" t="str" cm="1">
+        <f t="array" ref="P51">IF(SUM(COUNTIF(G51:N51, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>297</v>
       </c>
@@ -7088,9 +7075,9 @@
       <c r="O52" t="s">
         <v>396</v>
       </c>
-      <c r="P52" s="4" t="str" cm="1">
-        <f t="array" ref="P52">IF(SUM(COUNTIF(G52:N52, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P52" t="str" cm="1">
+        <f t="array" ref="P52">IF(SUM(COUNTIF(G52:N52, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7139,9 +7126,9 @@
       <c r="O53" t="s">
         <v>402</v>
       </c>
-      <c r="P53" s="4" t="str" cm="1">
-        <f t="array" ref="P53">IF(SUM(COUNTIF(G53:N53, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P53" t="str" cm="1">
+        <f t="array" ref="P53">IF(SUM(COUNTIF(G53:N53, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7190,8 +7177,8 @@
       <c r="O54" t="s">
         <v>397</v>
       </c>
-      <c r="P54" s="4" t="str" cm="1">
-        <f t="array" ref="P54">IF(SUM(COUNTIF(G54:N54, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P54" t="str" cm="1">
+        <f t="array" ref="P54">IF(SUM(COUNTIF(G54:N54, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -7241,12 +7228,12 @@
       <c r="O55" t="s">
         <v>402</v>
       </c>
-      <c r="P55" s="4" t="str" cm="1">
-        <f t="array" ref="P55">IF(SUM(COUNTIF(G55:N55, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P55" t="str" cm="1">
+        <f t="array" ref="P55">IF(SUM(COUNTIF(G55:N55, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>343</v>
       </c>
@@ -7292,9 +7279,9 @@
       <c r="O56" t="s">
         <v>398</v>
       </c>
-      <c r="P56" s="4" t="str" cm="1">
-        <f t="array" ref="P56">IF(SUM(COUNTIF(G56:N56, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P56" t="str" cm="1">
+        <f t="array" ref="P56">IF(SUM(COUNTIF(G56:N56, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7343,8 +7330,8 @@
       <c r="O57" t="s">
         <v>403</v>
       </c>
-      <c r="P57" s="4" t="str" cm="1">
-        <f t="array" ref="P57">IF(SUM(COUNTIF(G57:N57, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P57" t="str" cm="1">
+        <f t="array" ref="P57">IF(SUM(COUNTIF(G57:N57, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -7394,12 +7381,12 @@
       <c r="O58" t="s">
         <v>398</v>
       </c>
-      <c r="P58" s="4" t="str" cm="1">
-        <f t="array" ref="P58">IF(SUM(COUNTIF(G58:N58, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P58" t="str" cm="1">
+        <f t="array" ref="P58">IF(SUM(COUNTIF(G58:N58, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>83</v>
       </c>
@@ -7445,9 +7432,9 @@
       <c r="O59" t="s">
         <v>402</v>
       </c>
-      <c r="P59" s="4" t="str" cm="1">
-        <f t="array" ref="P59">IF(SUM(COUNTIF(G59:N59, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P59" t="str" cm="1">
+        <f t="array" ref="P59">IF(SUM(COUNTIF(G59:N59, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7496,12 +7483,12 @@
       <c r="O60" t="s">
         <v>395</v>
       </c>
-      <c r="P60" s="4" t="str" cm="1">
-        <f t="array" ref="P60">IF(SUM(COUNTIF(G60:N60, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P60" t="str" cm="1">
+        <f t="array" ref="P60">IF(SUM(COUNTIF(G60:N60, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>347</v>
       </c>
@@ -7547,12 +7534,12 @@
       <c r="O61" t="s">
         <v>398</v>
       </c>
-      <c r="P61" s="4" t="str" cm="1">
-        <f t="array" ref="P61">IF(SUM(COUNTIF(G61:N61, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P61" t="str" cm="1">
+        <f t="array" ref="P61">IF(SUM(COUNTIF(G61:N61, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -7598,9 +7585,9 @@
       <c r="O62" t="s">
         <v>401</v>
       </c>
-      <c r="P62" s="4" t="str" cm="1">
-        <f t="array" ref="P62">IF(SUM(COUNTIF(G62:N62, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P62" t="str" cm="1">
+        <f t="array" ref="P62">IF(SUM(COUNTIF(G62:N62, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7649,9 +7636,9 @@
       <c r="O63" t="s">
         <v>402</v>
       </c>
-      <c r="P63" s="4" t="str" cm="1">
-        <f t="array" ref="P63">IF(SUM(COUNTIF(G63:N63, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P63" t="str" cm="1">
+        <f t="array" ref="P63">IF(SUM(COUNTIF(G63:N63, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7700,9 +7687,9 @@
       <c r="O64" t="s">
         <v>403</v>
       </c>
-      <c r="P64" s="4" t="str" cm="1">
-        <f t="array" ref="P64">IF(SUM(COUNTIF(G64:N64, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P64" t="str" cm="1">
+        <f t="array" ref="P64">IF(SUM(COUNTIF(G64:N64, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7751,12 +7738,12 @@
       <c r="O65" t="s">
         <v>397</v>
       </c>
-      <c r="P65" s="4" t="str" cm="1">
-        <f t="array" ref="P65">IF(SUM(COUNTIF(G65:N65, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P65" t="str" cm="1">
+        <f t="array" ref="P65">IF(SUM(COUNTIF(G65:N65, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -7802,12 +7789,12 @@
       <c r="O66" t="s">
         <v>403</v>
       </c>
-      <c r="P66" s="4" t="str" cm="1">
-        <f t="array" ref="P66">IF(SUM(COUNTIF(G66:N66, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P66" t="str" cm="1">
+        <f t="array" ref="P66">IF(SUM(COUNTIF(G66:N66, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>300</v>
       </c>
@@ -7853,9 +7840,9 @@
       <c r="O67" t="s">
         <v>397</v>
       </c>
-      <c r="P67" s="4" t="str" cm="1">
-        <f t="array" ref="P67">IF(SUM(COUNTIF(G67:N67, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P67" t="str" cm="1">
+        <f t="array" ref="P67">IF(SUM(COUNTIF(G67:N67, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7904,9 +7891,9 @@
       <c r="O68" t="s">
         <v>395</v>
       </c>
-      <c r="P68" s="4" t="str" cm="1">
-        <f t="array" ref="P68">IF(SUM(COUNTIF(G68:N68, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P68" t="str" cm="1">
+        <f t="array" ref="P68">IF(SUM(COUNTIF(G68:N68, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -7955,8 +7942,8 @@
       <c r="O69" t="s">
         <v>395</v>
       </c>
-      <c r="P69" s="4" t="str" cm="1">
-        <f t="array" ref="P69">IF(SUM(COUNTIF(G69:N69, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P69" t="str" cm="1">
+        <f t="array" ref="P69">IF(SUM(COUNTIF(G69:N69, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -8006,12 +7993,12 @@
       <c r="O70" t="s">
         <v>395</v>
       </c>
-      <c r="P70" s="4" t="str" cm="1">
-        <f t="array" ref="P70">IF(SUM(COUNTIF(G70:N70, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P70" t="str" cm="1">
+        <f t="array" ref="P70">IF(SUM(COUNTIF(G70:N70, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>348</v>
       </c>
@@ -8057,9 +8044,9 @@
       <c r="O71" t="s">
         <v>398</v>
       </c>
-      <c r="P71" s="4" t="str" cm="1">
-        <f t="array" ref="P71">IF(SUM(COUNTIF(G71:N71, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P71" t="str" cm="1">
+        <f t="array" ref="P71">IF(SUM(COUNTIF(G71:N71, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8108,8 +8095,8 @@
       <c r="O72" t="s">
         <v>396</v>
       </c>
-      <c r="P72" s="4" t="str" cm="1">
-        <f t="array" ref="P72">IF(SUM(COUNTIF(G72:N72, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P72" t="str" cm="1">
+        <f t="array" ref="P72">IF(SUM(COUNTIF(G72:N72, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -8159,9 +8146,9 @@
       <c r="O73" t="s">
         <v>403</v>
       </c>
-      <c r="P73" s="4" t="str" cm="1">
-        <f t="array" ref="P73">IF(SUM(COUNTIF(G73:N73, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P73" t="str" cm="1">
+        <f t="array" ref="P73">IF(SUM(COUNTIF(G73:N73, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8210,12 +8197,12 @@
       <c r="O74" t="s">
         <v>398</v>
       </c>
-      <c r="P74" s="4" t="str" cm="1">
-        <f t="array" ref="P74">IF(SUM(COUNTIF(G74:N74, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P74" t="str" cm="1">
+        <f t="array" ref="P74">IF(SUM(COUNTIF(G74:N74, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -8261,12 +8248,12 @@
       <c r="O75" t="s">
         <v>402</v>
       </c>
-      <c r="P75" s="4" t="str" cm="1">
-        <f t="array" ref="P75">IF(SUM(COUNTIF(G75:N75, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P75" t="str" cm="1">
+        <f t="array" ref="P75">IF(SUM(COUNTIF(G75:N75, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>132</v>
       </c>
@@ -8312,9 +8299,9 @@
       <c r="O76" t="s">
         <v>403</v>
       </c>
-      <c r="P76" s="4" t="str" cm="1">
-        <f t="array" ref="P76">IF(SUM(COUNTIF(G76:N76, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P76" t="str" cm="1">
+        <f t="array" ref="P76">IF(SUM(COUNTIF(G76:N76, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8363,8 +8350,8 @@
       <c r="O77" t="s">
         <v>395</v>
       </c>
-      <c r="P77" s="4" t="str" cm="1">
-        <f t="array" ref="P77">IF(SUM(COUNTIF(G77:N77, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P77" t="str" cm="1">
+        <f t="array" ref="P77">IF(SUM(COUNTIF(G77:N77, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -8414,12 +8401,12 @@
       <c r="O78" t="s">
         <v>396</v>
       </c>
-      <c r="P78" s="4" t="str" cm="1">
-        <f t="array" ref="P78">IF(SUM(COUNTIF(G78:N78, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P78" t="str" cm="1">
+        <f t="array" ref="P78">IF(SUM(COUNTIF(G78:N78, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>318</v>
       </c>
@@ -8465,9 +8452,9 @@
       <c r="O79" t="s">
         <v>397</v>
       </c>
-      <c r="P79" s="4" t="str" cm="1">
-        <f t="array" ref="P79">IF(SUM(COUNTIF(G79:N79, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P79" t="str" cm="1">
+        <f t="array" ref="P79">IF(SUM(COUNTIF(G79:N79, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8516,12 +8503,12 @@
       <c r="O80" t="s">
         <v>396</v>
       </c>
-      <c r="P80" s="4" t="str" cm="1">
-        <f t="array" ref="P80">IF(SUM(COUNTIF(G80:N80, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P80" t="str" cm="1">
+        <f t="array" ref="P80">IF(SUM(COUNTIF(G80:N80, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>282</v>
       </c>
@@ -8567,9 +8554,9 @@
       <c r="O81" t="s">
         <v>396</v>
       </c>
-      <c r="P81" s="4" t="str" cm="1">
-        <f t="array" ref="P81">IF(SUM(COUNTIF(G81:N81, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P81" t="str" cm="1">
+        <f t="array" ref="P81">IF(SUM(COUNTIF(G81:N81, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8618,9 +8605,9 @@
       <c r="O82" t="s">
         <v>398</v>
       </c>
-      <c r="P82" s="4" t="str" cm="1">
-        <f t="array" ref="P82">IF(SUM(COUNTIF(G82:N82, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P82" t="str" cm="1">
+        <f t="array" ref="P82">IF(SUM(COUNTIF(G82:N82, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8669,8 +8656,8 @@
       <c r="O83" t="s">
         <v>403</v>
       </c>
-      <c r="P83" s="4" t="str" cm="1">
-        <f t="array" ref="P83">IF(SUM(COUNTIF(G83:N83, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P83" t="str" cm="1">
+        <f t="array" ref="P83">IF(SUM(COUNTIF(G83:N83, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -8720,8 +8707,8 @@
       <c r="O84" t="s">
         <v>403</v>
       </c>
-      <c r="P84" s="4" t="str" cm="1">
-        <f t="array" ref="P84">IF(SUM(COUNTIF(G84:N84, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P84" t="str" cm="1">
+        <f t="array" ref="P84">IF(SUM(COUNTIF(G84:N84, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -8771,8 +8758,8 @@
       <c r="O85" t="s">
         <v>395</v>
       </c>
-      <c r="P85" s="4" t="str" cm="1">
-        <f t="array" ref="P85">IF(SUM(COUNTIF(G85:N85, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P85" t="str" cm="1">
+        <f t="array" ref="P85">IF(SUM(COUNTIF(G85:N85, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -8822,9 +8809,9 @@
       <c r="O86" t="s">
         <v>395</v>
       </c>
-      <c r="P86" s="4" t="str" cm="1">
-        <f t="array" ref="P86">IF(SUM(COUNTIF(G86:N86, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P86" t="str" cm="1">
+        <f t="array" ref="P86">IF(SUM(COUNTIF(G86:N86, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8873,9 +8860,9 @@
       <c r="O87" t="s">
         <v>395</v>
       </c>
-      <c r="P87" s="4" t="str" cm="1">
-        <f t="array" ref="P87">IF(SUM(COUNTIF(G87:N87, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P87" t="str" cm="1">
+        <f t="array" ref="P87">IF(SUM(COUNTIF(G87:N87, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8924,9 +8911,9 @@
       <c r="O88" t="s">
         <v>395</v>
       </c>
-      <c r="P88" s="4" t="str" cm="1">
-        <f t="array" ref="P88">IF(SUM(COUNTIF(G88:N88, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P88" t="str" cm="1">
+        <f t="array" ref="P88">IF(SUM(COUNTIF(G88:N88, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -8975,12 +8962,12 @@
       <c r="O89" t="s">
         <v>395</v>
       </c>
-      <c r="P89" s="4" t="str" cm="1">
-        <f t="array" ref="P89">IF(SUM(COUNTIF(G89:N89, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P89" t="str" cm="1">
+        <f t="array" ref="P89">IF(SUM(COUNTIF(G89:N89, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>341</v>
       </c>
@@ -9026,9 +9013,9 @@
       <c r="O90" t="s">
         <v>398</v>
       </c>
-      <c r="P90" s="4" t="str" cm="1">
-        <f t="array" ref="P90">IF(SUM(COUNTIF(G90:N90, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P90" t="str" cm="1">
+        <f t="array" ref="P90">IF(SUM(COUNTIF(G90:N90, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -9077,12 +9064,12 @@
       <c r="O91" t="s">
         <v>402</v>
       </c>
-      <c r="P91" s="4" t="str" cm="1">
-        <f t="array" ref="P91">IF(SUM(COUNTIF(G91:N91, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P91" t="str" cm="1">
+        <f t="array" ref="P91">IF(SUM(COUNTIF(G91:N91, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>226</v>
       </c>
@@ -9128,9 +9115,9 @@
       <c r="O92" t="s">
         <v>395</v>
       </c>
-      <c r="P92" s="4" t="str" cm="1">
-        <f t="array" ref="P92">IF(SUM(COUNTIF(G92:N92, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P92" t="str" cm="1">
+        <f t="array" ref="P92">IF(SUM(COUNTIF(G92:N92, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -9179,12 +9166,12 @@
       <c r="O93" t="s">
         <v>395</v>
       </c>
-      <c r="P93" s="4" t="str" cm="1">
-        <f t="array" ref="P93">IF(SUM(COUNTIF(G93:N93, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P93" t="str" cm="1">
+        <f t="array" ref="P93">IF(SUM(COUNTIF(G93:N93, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>334</v>
       </c>
@@ -9230,12 +9217,12 @@
       <c r="O94" t="s">
         <v>397</v>
       </c>
-      <c r="P94" s="4" t="str" cm="1">
-        <f t="array" ref="P94">IF(SUM(COUNTIF(G94:N94, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P94" t="str" cm="1">
+        <f t="array" ref="P94">IF(SUM(COUNTIF(G94:N94, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>72</v>
       </c>
@@ -9281,9 +9268,9 @@
       <c r="O95" t="s">
         <v>402</v>
       </c>
-      <c r="P95" s="4" t="str" cm="1">
-        <f t="array" ref="P95">IF(SUM(COUNTIF(G95:N95, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P95" t="str" cm="1">
+        <f t="array" ref="P95">IF(SUM(COUNTIF(G95:N95, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -9332,8 +9319,8 @@
       <c r="O96" t="s">
         <v>402</v>
       </c>
-      <c r="P96" s="4" t="str" cm="1">
-        <f t="array" ref="P96">IF(SUM(COUNTIF(G96:N96, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P96" t="str" cm="1">
+        <f t="array" ref="P96">IF(SUM(COUNTIF(G96:N96, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9383,12 +9370,12 @@
       <c r="O97" t="s">
         <v>398</v>
       </c>
-      <c r="P97" s="4" t="str" cm="1">
-        <f t="array" ref="P97">IF(SUM(COUNTIF(G97:N97, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P97" t="str" cm="1">
+        <f t="array" ref="P97">IF(SUM(COUNTIF(G97:N97, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>136</v>
       </c>
@@ -9434,12 +9421,12 @@
       <c r="O98" t="s">
         <v>403</v>
       </c>
-      <c r="P98" s="4" t="str" cm="1">
-        <f t="array" ref="P98">IF(SUM(COUNTIF(G98:N98, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P98" t="str" cm="1">
+        <f t="array" ref="P98">IF(SUM(COUNTIF(G98:N98, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>79</v>
       </c>
@@ -9485,9 +9472,9 @@
       <c r="O99" t="s">
         <v>402</v>
       </c>
-      <c r="P99" s="4" t="str" cm="1">
-        <f t="array" ref="P99">IF(SUM(COUNTIF(G99:N99, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P99" t="str" cm="1">
+        <f t="array" ref="P99">IF(SUM(COUNTIF(G99:N99, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -9536,8 +9523,8 @@
       <c r="O100" t="s">
         <v>403</v>
       </c>
-      <c r="P100" s="4" t="str" cm="1">
-        <f t="array" ref="P100">IF(SUM(COUNTIF(G100:N100, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P100" t="str" cm="1">
+        <f t="array" ref="P100">IF(SUM(COUNTIF(G100:N100, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9587,8 +9574,8 @@
       <c r="O101" t="s">
         <v>395</v>
       </c>
-      <c r="P101" s="4" t="str" cm="1">
-        <f t="array" ref="P101">IF(SUM(COUNTIF(G101:N101, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P101" t="str" cm="1">
+        <f t="array" ref="P101">IF(SUM(COUNTIF(G101:N101, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9638,8 +9625,8 @@
       <c r="O102" t="s">
         <v>395</v>
       </c>
-      <c r="P102" s="4" t="str" cm="1">
-        <f t="array" ref="P102">IF(SUM(COUNTIF(G102:N102, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P102" t="str" cm="1">
+        <f t="array" ref="P102">IF(SUM(COUNTIF(G102:N102, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9689,12 +9676,12 @@
       <c r="O103" t="s">
         <v>403</v>
       </c>
-      <c r="P103" s="4" t="str" cm="1">
-        <f t="array" ref="P103">IF(SUM(COUNTIF(G103:N103, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P103" t="str" cm="1">
+        <f t="array" ref="P103">IF(SUM(COUNTIF(G103:N103, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>358</v>
       </c>
@@ -9740,8 +9727,8 @@
       <c r="O104" t="s">
         <v>398</v>
       </c>
-      <c r="P104" s="4" t="str" cm="1">
-        <f t="array" ref="P104">IF(SUM(COUNTIF(G104:N104, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P104" t="str" cm="1">
+        <f t="array" ref="P104">IF(SUM(COUNTIF(G104:N104, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9791,8 +9778,8 @@
       <c r="O105" t="s">
         <v>402</v>
       </c>
-      <c r="P105" s="4" t="str" cm="1">
-        <f t="array" ref="P105">IF(SUM(COUNTIF(G105:N105, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P105" t="str" cm="1">
+        <f t="array" ref="P105">IF(SUM(COUNTIF(G105:N105, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9842,8 +9829,8 @@
       <c r="O106" t="s">
         <v>396</v>
       </c>
-      <c r="P106" s="4" t="str" cm="1">
-        <f t="array" ref="P106">IF(SUM(COUNTIF(G106:N106, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P106" t="str" cm="1">
+        <f t="array" ref="P106">IF(SUM(COUNTIF(G106:N106, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9893,8 +9880,8 @@
       <c r="O107" t="s">
         <v>397</v>
       </c>
-      <c r="P107" s="4" t="str" cm="1">
-        <f t="array" ref="P107">IF(SUM(COUNTIF(G107:N107, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P107" t="str" cm="1">
+        <f t="array" ref="P107">IF(SUM(COUNTIF(G107:N107, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9944,8 +9931,8 @@
       <c r="O108" t="s">
         <v>402</v>
       </c>
-      <c r="P108" s="4" t="str" cm="1">
-        <f t="array" ref="P108">IF(SUM(COUNTIF(G108:N108, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P108" t="str" cm="1">
+        <f t="array" ref="P108">IF(SUM(COUNTIF(G108:N108, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -9995,9 +9982,9 @@
       <c r="O109" t="s">
         <v>397</v>
       </c>
-      <c r="P109" s="4" t="str" cm="1">
-        <f t="array" ref="P109">IF(SUM(COUNTIF(G109:N109, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P109" t="str" cm="1">
+        <f t="array" ref="P109">IF(SUM(COUNTIF(G109:N109, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -10046,12 +10033,12 @@
       <c r="O110" t="s">
         <v>398</v>
       </c>
-      <c r="P110" s="4" t="str" cm="1">
-        <f t="array" ref="P110">IF(SUM(COUNTIF(G110:N110, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+      <c r="P110" t="str" cm="1">
+        <f t="array" ref="P110">IF(SUM(COUNTIF(G110:N110, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>373</v>
       </c>
@@ -10097,8 +10084,8 @@
       <c r="O111" t="s">
         <v>398</v>
       </c>
-      <c r="P111" s="4" t="str" cm="1">
-        <f t="array" ref="P111">IF(SUM(COUNTIF(G111:N111, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P111" t="str" cm="1">
+        <f t="array" ref="P111">IF(SUM(COUNTIF(G111:N111, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10148,9 +10135,9 @@
       <c r="O112" t="s">
         <v>403</v>
       </c>
-      <c r="P112" s="4" t="str" cm="1">
-        <f t="array" ref="P112">IF(SUM(COUNTIF(G112:N112, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P112" t="str" cm="1">
+        <f t="array" ref="P112">IF(SUM(COUNTIF(G112:N112, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -10199,8 +10186,8 @@
       <c r="O113" t="s">
         <v>402</v>
       </c>
-      <c r="P113" s="4" t="str" cm="1">
-        <f t="array" ref="P113">IF(SUM(COUNTIF(G113:N113, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P113" t="str" cm="1">
+        <f t="array" ref="P113">IF(SUM(COUNTIF(G113:N113, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10250,8 +10237,8 @@
       <c r="O114" t="s">
         <v>398</v>
       </c>
-      <c r="P114" s="4" t="str" cm="1">
-        <f t="array" ref="P114">IF(SUM(COUNTIF(G114:N114, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P114" t="str" cm="1">
+        <f t="array" ref="P114">IF(SUM(COUNTIF(G114:N114, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10301,8 +10288,8 @@
       <c r="O115" t="s">
         <v>402</v>
       </c>
-      <c r="P115" s="4" t="str" cm="1">
-        <f t="array" ref="P115">IF(SUM(COUNTIF(G115:N115, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P115" t="str" cm="1">
+        <f t="array" ref="P115">IF(SUM(COUNTIF(G115:N115, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10352,8 +10339,8 @@
       <c r="O116" t="s">
         <v>403</v>
       </c>
-      <c r="P116" s="4" t="str" cm="1">
-        <f t="array" ref="P116">IF(SUM(COUNTIF(G116:N116, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P116" t="str" cm="1">
+        <f t="array" ref="P116">IF(SUM(COUNTIF(G116:N116, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10403,8 +10390,8 @@
       <c r="O117" t="s">
         <v>398</v>
       </c>
-      <c r="P117" s="4" t="str" cm="1">
-        <f t="array" ref="P117">IF(SUM(COUNTIF(G117:N117, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P117" t="str" cm="1">
+        <f t="array" ref="P117">IF(SUM(COUNTIF(G117:N117, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10454,8 +10441,8 @@
       <c r="O118" t="s">
         <v>395</v>
       </c>
-      <c r="P118" s="4" t="str" cm="1">
-        <f t="array" ref="P118">IF(SUM(COUNTIF(G118:N118, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P118" t="str" cm="1">
+        <f t="array" ref="P118">IF(SUM(COUNTIF(G118:N118, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10505,8 +10492,8 @@
       <c r="O119" t="s">
         <v>398</v>
       </c>
-      <c r="P119" s="4" t="str" cm="1">
-        <f t="array" ref="P119">IF(SUM(COUNTIF(G119:N119, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P119" t="str" cm="1">
+        <f t="array" ref="P119">IF(SUM(COUNTIF(G119:N119, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10556,8 +10543,8 @@
       <c r="O120" t="s">
         <v>403</v>
       </c>
-      <c r="P120" s="4" t="str" cm="1">
-        <f t="array" ref="P120">IF(SUM(COUNTIF(G120:N120, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P120" t="str" cm="1">
+        <f t="array" ref="P120">IF(SUM(COUNTIF(G120:N120, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10607,8 +10594,8 @@
       <c r="O121" t="s">
         <v>398</v>
       </c>
-      <c r="P121" s="4" t="str" cm="1">
-        <f t="array" ref="P121">IF(SUM(COUNTIF(G121:N121, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P121" t="str" cm="1">
+        <f t="array" ref="P121">IF(SUM(COUNTIF(G121:N121, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10658,8 +10645,8 @@
       <c r="O122" t="s">
         <v>403</v>
       </c>
-      <c r="P122" s="4" t="str" cm="1">
-        <f t="array" ref="P122">IF(SUM(COUNTIF(G122:N122, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P122" t="str" cm="1">
+        <f t="array" ref="P122">IF(SUM(COUNTIF(G122:N122, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10709,8 +10696,8 @@
       <c r="O123" t="s">
         <v>403</v>
       </c>
-      <c r="P123" s="4" t="str" cm="1">
-        <f t="array" ref="P123">IF(SUM(COUNTIF(G123:N123, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P123" t="str" cm="1">
+        <f t="array" ref="P123">IF(SUM(COUNTIF(G123:N123, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10760,8 +10747,8 @@
       <c r="O124" t="s">
         <v>403</v>
       </c>
-      <c r="P124" s="4" t="str" cm="1">
-        <f t="array" ref="P124">IF(SUM(COUNTIF(G124:N124, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P124" t="str" cm="1">
+        <f t="array" ref="P124">IF(SUM(COUNTIF(G124:N124, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10811,8 +10798,8 @@
       <c r="O125" t="s">
         <v>395</v>
       </c>
-      <c r="P125" s="4" t="str" cm="1">
-        <f t="array" ref="P125">IF(SUM(COUNTIF(G125:N125, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P125" t="str" cm="1">
+        <f t="array" ref="P125">IF(SUM(COUNTIF(G125:N125, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>
@@ -10862,12 +10849,12 @@
       <c r="O126" t="s">
         <v>395</v>
       </c>
-      <c r="P126" s="4" t="str" cm="1">
-        <f t="array" ref="P126">IF(SUM(COUNTIF(G126:N126, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Hide</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P126" t="str" cm="1">
+        <f t="array" ref="P126">IF(SUM(COUNTIF(G126:N126, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>210</v>
       </c>
@@ -10913,9 +10900,9 @@
       <c r="O127" t="s">
         <v>395</v>
       </c>
-      <c r="P127" s="4" t="str" cm="1">
-        <f t="array" ref="P127">IF(SUM(COUNTIF(G127:N127, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
-        <v>Show</v>
+      <c r="P127" t="str" cm="1">
+        <f t="array" ref="P127">IF(SUM(COUNTIF(G127:N127, {""}))&gt;0, "Show", "Hide")</f>
+        <v>Hide</v>
       </c>
     </row>
     <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
@@ -10964,8 +10951,8 @@
       <c r="O128" t="s">
         <v>395</v>
       </c>
-      <c r="P128" s="4" t="str" cm="1">
-        <f t="array" ref="P128">IF(SUM(COUNTIF(G128:N128, {"CakeAssault","Sam","Dank Fornasty"}))&gt;0, "Show", "Hide")</f>
+      <c r="P128" t="str" cm="1">
+        <f t="array" ref="P128">IF(SUM(COUNTIF(G128:N128, {""}))&gt;0, "Show", "Hide")</f>
         <v>Hide</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished all ranking entries
</commit_message>
<xml_diff>
--- a/data/Rivals1TournamentsAnalysis.xlsx
+++ b/data/Rivals1TournamentsAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlmon\Documents\GitHub\rivals-blog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A8F47D-C1F1-43CF-A49D-3FD80A04768F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB74F01D-845D-4E13-9699-974AD56C1882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{40EF91EA-8845-4BB8-88F3-89A70BCD1D65}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{40EF91EA-8845-4BB8-88F3-89A70BCD1D65}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournaments" sheetId="1" r:id="rId1"/>
@@ -4048,7 +4048,7 @@
   <autoFilter ref="A1:P128" xr:uid="{ACAD4DCB-C46A-43E3-A436-186B1BC8423B}">
     <filterColumn colId="6">
       <filters>
-        <filter val="Blue"/>
+        <filter val="Soulrifle211"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4399,7 +4399,7 @@
   <dimension ref="A1:R128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5040,7 +5040,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>388</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>347</v>
       </c>
@@ -9630,7 +9630,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>152</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>358</v>
       </c>
@@ -10038,7 +10038,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>373</v>
       </c>
@@ -10293,7 +10293,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>170</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>179</v>
       </c>
@@ -11155,7 +11155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D4FAA9-90ED-40C0-BFF3-3F56EA39CFBA}">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update tournament analysis spreadsheet
</commit_message>
<xml_diff>
--- a/data/Rivals1TournamentsAnalysis.xlsx
+++ b/data/Rivals1TournamentsAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlmon\Documents\GitHub\rivals-blog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB74F01D-845D-4E13-9699-974AD56C1882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C568E4-C269-44EC-86F1-605685398B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{40EF91EA-8845-4BB8-88F3-89A70BCD1D65}"/>
   </bookViews>
@@ -4048,7 +4048,7 @@
   <autoFilter ref="A1:P128" xr:uid="{ACAD4DCB-C46A-43E3-A436-186B1BC8423B}">
     <filterColumn colId="6">
       <filters>
-        <filter val="Soulrifle211"/>
+        <filter val="Xaro"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="R1">
         <f>SUBTOTAL(3, A2:A200)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
@@ -4581,7 +4581,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>390</v>
       </c>
@@ -4887,7 +4887,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>387</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>339</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>350</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -9630,7 +9630,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>152</v>
       </c>
@@ -10293,7 +10293,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>170</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>Hide</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>179</v>
       </c>

</xml_diff>